<commit_message>
Rework Lifting Gear Manager #2
</commit_message>
<xml_diff>
--- a/files/system/import-lashing-sample.xlsx
+++ b/files/system/import-lashing-sample.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t xml:space="preserve">No</t>
   </si>
@@ -52,6 +52,12 @@
     <t xml:space="preserve">BL</t>
   </si>
   <si>
+    <t xml:space="preserve">ICC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manufacturer</t>
+  </si>
+  <si>
     <t xml:space="preserve">Supplied Place</t>
   </si>
   <si>
@@ -80,6 +86,12 @@
   </si>
   <si>
     <t xml:space="preserve">with hook</t>
+  </si>
+  <si>
+    <t xml:space="preserve">White/Blue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seil-Heiring</t>
   </si>
   <si>
     <t xml:space="preserve">Hamburg</t>
@@ -106,7 +118,7 @@
     <numFmt numFmtId="165" formatCode="00"/>
     <numFmt numFmtId="166" formatCode="[$-809]dd\ mmm\ yyyy;@"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -178,12 +190,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF44546A"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -303,7 +309,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -314,6 +320,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -360,27 +370,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -550,7 +552,7 @@
   <dimension ref="A1:AMJ6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
+      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K:K"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -565,73 +567,79 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="8.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="8.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="8.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="12.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="2" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="12.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="17.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="10.69"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1013" min="18" style="2" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="8.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="3" width="11.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="12.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="2" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="12.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="17.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="10.69"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="20" style="2" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+    <row r="1" s="5" customFormat="true" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="ALZ1" s="5"/>
-      <c r="AMA1" s="5"/>
-      <c r="AMB1" s="5"/>
-      <c r="AMC1" s="5"/>
-      <c r="AMD1" s="0"/>
-      <c r="AME1" s="0"/>
+      <c r="R1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="AMB1" s="6"/>
+      <c r="AMC1" s="6"/>
+      <c r="AMD1" s="6"/>
+      <c r="AME1" s="6"/>
       <c r="AMF1" s="0"/>
       <c r="AMG1" s="0"/>
       <c r="AMH1" s="0"/>
@@ -639,84 +647,90 @@
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="n">
+      <c r="A2" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="10" t="n">
+      <c r="C2" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="11" t="n">
         <v>50</v>
       </c>
-      <c r="F2" s="11" t="n">
+      <c r="F2" s="12" t="n">
         <v>6000</v>
       </c>
-      <c r="G2" s="12" t="n">
+      <c r="G2" s="13" t="n">
         <v>250</v>
       </c>
-      <c r="H2" s="13" t="n">
+      <c r="H2" s="14" t="n">
         <v>1500</v>
       </c>
-      <c r="I2" s="12" t="n">
+      <c r="I2" s="13" t="n">
         <v>200</v>
       </c>
-      <c r="J2" s="12" t="n">
+      <c r="J2" s="13" t="n">
         <v>350</v>
       </c>
-      <c r="K2" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="M2" s="16" t="s">
+      <c r="K2" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="N2" s="17" t="n">
+      <c r="L2" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="P2" s="15" t="n">
         <v>44891</v>
       </c>
-      <c r="O2" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="P2" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q2" s="16" t="n">
+      <c r="Q2" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="R2" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="S2" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="R2" s="0"/>
-      <c r="S2" s="0"/>
       <c r="T2" s="0"/>
+      <c r="U2" s="0"/>
+      <c r="V2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
+      <c r="B4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
+      <c r="B5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
+      <c r="B6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">

</xml_diff>